<commit_message>
add documento de evolutiva.
</commit_message>
<xml_diff>
--- a/03 - Analise/Docs/Evolutivas/Evolutiva_12082013.xlsx
+++ b/03 - Analise/Docs/Evolutivas/Evolutiva_12082013.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Cod. Erro</t>
   </si>
@@ -87,13 +87,7 @@
     <t xml:space="preserve">Criar status para venda e compra, em aberto e finalizado. Permitir editar somente as vendas em aberto. Ver como vai ficar essa lógica. Em aberto porque o funcionário pode alterar a venda mais tarde. Sinalizar com um botão verde(status em aberto) e Amarelo(status finalizado). </t>
   </si>
   <si>
-    <t>8h</t>
-  </si>
-  <si>
     <t>Moderado</t>
-  </si>
-  <si>
-    <t>72h</t>
   </si>
   <si>
     <t xml:space="preserve">3- Criar uma tela para forma de pagamento com os seguintes campos: Dinheiro, Bônus, Cheque1, data liberação cheque1, Cheque2, data liberação cheque 2.  Nessa tela ao confirmar a forma de pagamento validar a aprovação da venda.O calculo da data será alterado, será em feito em cima das datas colocadas nessa nova tela ao invés de sempre considera 30 e 60 dias. Na tela Venda retirar o combo de forma pagamento e colocar um botão para chamar a tela acima.
@@ -103,29 +97,32 @@
     <t>4-Na tela de revendedor colocar um botão ao lado do campo limite em uso. Esse botão vai exibir o histórico das valores a liberar, exibir numa grid com as colunas valor e data a liberar. Ex: Valor R$ 100,00 - Data 04/082013, Valor R$ 120,00 - Data 18/08/2013.</t>
   </si>
   <si>
-    <t>4h</t>
-  </si>
-  <si>
     <t>E006</t>
   </si>
   <si>
     <t>Adicionar mais um dígito no telefone</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
     <t>Como implementar</t>
   </si>
   <si>
     <t>Na tela consulta revendedor adicionar filtros: CEP, Cidade, Bairro e Telefone. Lembrar buscar por proximidade como é feito por código.</t>
+  </si>
+  <si>
+    <t>Valor Hora</t>
+  </si>
+  <si>
+    <t>Data Entrega</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +135,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,10 +175,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -188,11 +198,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -224,7 +294,7 @@
   <autoFilter ref="B4:E12"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Cod. Erro"/>
-    <tableColumn id="2" name="Descrição Erro" dataDxfId="1"/>
+    <tableColumn id="2" name="Descrição Erro" dataDxfId="6"/>
     <tableColumn id="3" name="Nível"/>
     <tableColumn id="4" name="Num. Horas"/>
   </tableColumns>
@@ -233,16 +303,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B4:F19" totalsRowShown="0">
-  <autoFilter ref="B4:F19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B4:F20" totalsRowCount="1">
+  <autoFilter ref="B4:F20">
     <filterColumn colId="2"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Cod. Evolutiva"/>
-    <tableColumn id="2" name="Descrição Evolutiva"/>
-    <tableColumn id="5" name="Como implementar" dataDxfId="0"/>
-    <tableColumn id="3" name="Nível"/>
-    <tableColumn id="4" name="Num Horas"/>
+    <tableColumn id="1" name="Cod. Evolutiva" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Descrição Evolutiva" totalsRowDxfId="3"/>
+    <tableColumn id="5" name="Como implementar" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Nível" totalsRowDxfId="1"/>
+    <tableColumn id="4" name="Num Horas" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(F5:F10)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -651,10 +723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:F17"/>
+  <dimension ref="B4:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,9 +737,12 @@
     <col min="4" max="4" width="51.140625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:10">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -675,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -683,8 +758,14 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="29.25">
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="29.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -695,11 +776,21 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="43.5">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3</v>
+      </c>
+      <c r="I5" s="8">
+        <f>H5*Tabela2[[#Totals],[Num Horas]]</f>
+        <v>279</v>
+      </c>
+      <c r="J5" s="11">
+        <v>41579</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="43.5">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -710,97 +801,107 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="99.75">
+      <c r="F6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="99.75">
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="43.5">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="43.5">
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="29.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="29.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:10">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:10">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:10">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:10">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:10">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="2:6">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9">
+        <f>SUM(F5:F10)</f>
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Alterando arquivo de Evolutiva_12082013.xlsx;
</commit_message>
<xml_diff>
--- a/03 - Analise/Docs/Evolutivas/Evolutiva_12082013.xlsx
+++ b/03 - Analise/Docs/Evolutivas/Evolutiva_12082013.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Cod. Erro</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Data Entrega</t>
+  </si>
+  <si>
+    <t>Depois que usuário entrar com o valor pedido escrito comparar com o valor total com desconto se for diferente exiber uma popup com um mensagem de alerta assim: "O Valor do pedido escrito está diferente do valor total com desconto, deseja continuar?" exibir os botões sim e não.</t>
+  </si>
+  <si>
+    <t>Criar atributo statusPedido do tipo int na classe Pedido. Criar coluna status_pedido do tipo Int na tabela tb_pedido. Nas telas de pedido adicionar comobox situação do pedido com valor default "Em Aberto".  Ao Salvar o pedido lembrar o usuário o status do pedido para que ele possa finalizar a venda ou então deixa-lá em aberto.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +310,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B4:F20" totalsRowCount="1">
-  <autoFilter ref="B4:F20">
+  <autoFilter ref="B4:F19">
     <filterColumn colId="2"/>
   </autoFilter>
   <tableColumns count="5">
@@ -725,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,14 +771,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="29.25">
+    <row r="5" spans="2:10" ht="86.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
@@ -790,14 +798,16 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="43.5">
+    <row r="6" spans="2:10" ht="100.5">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>

</xml_diff>